<commit_message>
Modifications of ovw demo sheets
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVMDemo-RProductListing.xlsx
+++ b/docs/OVW Sheets/OVMDemo-RProductListing.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\OVW Migration Project\Project Code\OVWMigration\docs\OVW Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration Dec 28\OVWMigration\docs\OVW Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="24000" windowHeight="9675" firstSheet="26" activeTab="38"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="24000" windowHeight="9675" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="en_au" sheetId="1" r:id="rId1"/>
@@ -25,32 +25,34 @@
     <sheet name="fr_ch" sheetId="10" r:id="rId11"/>
     <sheet name="de_de" sheetId="11" r:id="rId12"/>
     <sheet name="da_dk" sheetId="12" r:id="rId13"/>
-    <sheet name="fr_dz" sheetId="14" r:id="rId14"/>
-    <sheet name="es_es" sheetId="15" r:id="rId15"/>
-    <sheet name="fr_fr" sheetId="16" r:id="rId16"/>
-    <sheet name="en_hk" sheetId="17" r:id="rId17"/>
-    <sheet name="zh_hk" sheetId="18" r:id="rId18"/>
-    <sheet name="en_il" sheetId="19" r:id="rId19"/>
-    <sheet name="en_in" sheetId="20" r:id="rId20"/>
-    <sheet name="it_it" sheetId="21" r:id="rId21"/>
-    <sheet name="ko_kr" sheetId="22" r:id="rId22"/>
-    <sheet name="en_ae" sheetId="24" r:id="rId23"/>
-    <sheet name="ar_ae" sheetId="25" r:id="rId24"/>
-    <sheet name="nl_nl" sheetId="26" r:id="rId25"/>
-    <sheet name="no_no" sheetId="27" r:id="rId26"/>
-    <sheet name="pl_pl" sheetId="28" r:id="rId27"/>
-    <sheet name="pt_pt" sheetId="29" r:id="rId28"/>
-    <sheet name="ru_ru" sheetId="30" r:id="rId29"/>
-    <sheet name="sv_se" sheetId="31" r:id="rId30"/>
-    <sheet name="en_sg" sheetId="32" r:id="rId31"/>
-    <sheet name="th_th" sheetId="33" r:id="rId32"/>
-    <sheet name="tr_tr" sheetId="34" r:id="rId33"/>
-    <sheet name="zh_tw" sheetId="35" r:id="rId34"/>
-    <sheet name="ru_ua" sheetId="36" r:id="rId35"/>
-    <sheet name="en_gb" sheetId="37" r:id="rId36"/>
-    <sheet name="en_za" sheetId="38" r:id="rId37"/>
-    <sheet name="zh_cn" sheetId="39" r:id="rId38"/>
-    <sheet name="ja_jp" sheetId="40" r:id="rId39"/>
+    <sheet name="en_dz" sheetId="45" r:id="rId14"/>
+    <sheet name="fr_dz" sheetId="14" r:id="rId15"/>
+    <sheet name="es_es" sheetId="15" r:id="rId16"/>
+    <sheet name="fr_fr" sheetId="16" r:id="rId17"/>
+    <sheet name="en_hk" sheetId="17" r:id="rId18"/>
+    <sheet name="zh_hk" sheetId="18" r:id="rId19"/>
+    <sheet name="en_il" sheetId="19" r:id="rId20"/>
+    <sheet name="en_in" sheetId="20" r:id="rId21"/>
+    <sheet name="it_it" sheetId="21" r:id="rId22"/>
+    <sheet name="ko_kr" sheetId="22" r:id="rId23"/>
+    <sheet name="en_ae" sheetId="24" r:id="rId24"/>
+    <sheet name="ar_ae" sheetId="25" r:id="rId25"/>
+    <sheet name="nl_nl" sheetId="26" r:id="rId26"/>
+    <sheet name="no_no" sheetId="27" r:id="rId27"/>
+    <sheet name="pl_pl" sheetId="28" r:id="rId28"/>
+    <sheet name="pt_pt" sheetId="29" r:id="rId29"/>
+    <sheet name="ru_ru" sheetId="30" r:id="rId30"/>
+    <sheet name="es_mx" sheetId="43" r:id="rId31"/>
+    <sheet name="sv_se" sheetId="31" r:id="rId32"/>
+    <sheet name="en_sg" sheetId="32" r:id="rId33"/>
+    <sheet name="th_th" sheetId="33" r:id="rId34"/>
+    <sheet name="tr_tr" sheetId="34" r:id="rId35"/>
+    <sheet name="zh_tw" sheetId="35" r:id="rId36"/>
+    <sheet name="ru_ua" sheetId="36" r:id="rId37"/>
+    <sheet name="en_gb" sheetId="37" r:id="rId38"/>
+    <sheet name="en_za" sheetId="38" r:id="rId39"/>
+    <sheet name="zh_cn" sheetId="39" r:id="rId40"/>
+    <sheet name="ja_jp" sheetId="40" r:id="rId41"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="199">
   <si>
     <t>http://www.cisco.com/web/ANZ/products/routers/products.html</t>
   </si>
@@ -413,6 +415,252 @@
   </si>
   <si>
     <t>wireless</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/products/unified_computing/products.html</t>
+  </si>
+  <si>
+    <t>servers-unified-computing</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DE/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>storage-networking</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/products/products_netsol/ucs/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CN/products/products_netsol/storage_networking/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/products/unified_computing/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/cisco/web/UK/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/productos/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/LA/productos/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/produtos/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/produtos/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/ar/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/product/hs/ucs/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/JP/product/hs/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/FR/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/nl/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/nl/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/products/unified_computing/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/products/unified_computing/products_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CA/products/storage/products_fr.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/de/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/de/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/fr/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/CH/fr/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DK/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/DK/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/products/FR/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/EA/products/FR/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ES/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ES/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/tc/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/HK/tc/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IL/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IL/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/products/unified_computing/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IN/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IT/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/IT/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/products/pc/unified_computing/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/KR/products/pc/snp/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ME/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NL/producten/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NL/producten/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NO/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/NO/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PL/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PL/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PT/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PT/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SE/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SE/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SG/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/SG/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TH/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TH/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TR/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TR/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TW/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/TW/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/UA/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/UA/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ZA/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ZA/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/products/unified_computing/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ANZ/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/AT/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/AT/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/fr/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BE/fr/products/storage/products.html</t>
   </si>
 </sst>
 </file>
@@ -779,13 +1027,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -823,10 +1071,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -836,9 +1100,11 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -847,7 +1113,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,10 +1157,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -904,6 +1186,8 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -914,12 +1198,12 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -958,10 +1242,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -971,6 +1271,8 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -978,15 +1280,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1024,11 +1326,35 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1039,7 +1365,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,10 +1409,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1096,6 +1438,8 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1103,10 +1447,56 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,27 +1539,51 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.42578125" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1208,10 +1622,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -1221,22 +1651,24 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A1" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.140625" customWidth="1"/>
+    <col min="1" max="1" width="60.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1275,10 +1707,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1288,22 +1736,24 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.42578125" customWidth="1"/>
+    <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1342,10 +1792,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1355,17 +1821,19 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,10 +1877,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -1422,70 +1906,8 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="66.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1496,7 +1918,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,10 +1962,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -1553,6 +1991,8 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1560,15 +2000,97 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1606,22 +2128,46 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5" display="http://www.cisco.com/web/IN/products/unified_computing/services.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,27 +2210,51 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1722,22 +2292,46 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4" display="http://www.cisco.com/web/KR/products/pc/unified_computing/services.html"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,22 +2374,46 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,27 +2456,51 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4" display="http://www.cisco.com/web/ME/ar/products/storage/index.html"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.7109375" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1896,22 +2538,46 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,22 +2620,46 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2012,27 +2702,51 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.140625" customWidth="1"/>
+    <col min="1" max="1" width="60.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2070,78 +2784,35 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="74.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2152,7 +2823,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,10 +2867,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -2209,6 +2896,8 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2216,15 +2905,146 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.7109375" customWidth="1"/>
+    <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2262,27 +3082,51 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2321,10 +3165,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -2334,22 +3194,24 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" customWidth="1"/>
+    <col min="1" max="1" width="60.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2387,27 +3249,51 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67" customWidth="1"/>
+    <col min="1" max="1" width="60.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2446,10 +3332,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -2459,22 +3361,24 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.7109375" customWidth="1"/>
+    <col min="1" max="1" width="61.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2512,27 +3416,51 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.42578125" customWidth="1"/>
+    <col min="1" max="1" width="61.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2570,29 +3498,53 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2628,22 +3580,46 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4" display="http://www.cisco.com/cisco/web/UK/products/unified_computing/services.html"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2686,22 +3662,131 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2744,27 +3829,51 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.28515625" customWidth="1"/>
+    <col min="1" max="1" width="62.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2802,78 +3911,35 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="68.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2884,12 +3950,12 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2928,10 +3994,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -2941,6 +4023,8 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2980,7 +4064,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2991,7 +4075,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
@@ -3024,10 +4108,26 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -3037,6 +4137,8 @@
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3047,7 +4149,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3091,16 +4193,34 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3108,15 +4228,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3154,11 +4274,35 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>